<commit_message>
Adding revised paper for rebuttal
</commit_message>
<xml_diff>
--- a/Results/Graphs in Paper/getScores.xlsx
+++ b/Results/Graphs in Paper/getScores.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/arcchit/eclipse-workspace/OpenProbFOIL/Checks/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/arcchit/Docs/safeLearner/Results/Graphs in Paper/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE9202C3-4127-5D41-AFE4-8FD565034F14}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4628AC72-FCA4-B04F-A14E-F10BC700F964}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="780" yWindow="560" windowWidth="27640" windowHeight="16940" activeTab="4" xr2:uid="{59EC3011-7FAF-0E4C-AC49-706653CD767F}"/>
   </bookViews>
@@ -19,16 +19,10 @@
     <sheet name="Squared Loss" sheetId="4" r:id="rId4"/>
     <sheet name="Sheet1" sheetId="5" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="179021"/>
-  <fileRecoveryPr repairLoad="1"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -5146,7 +5140,7 @@
                 <a:effectLst/>
               </c:spPr>
               <c:txPr>
-                <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
                   <a:spAutoFit/>
                 </a:bodyPr>
                 <a:lstStyle/>
@@ -5347,7 +5341,7 @@
                 <a:effectLst/>
               </c:spPr>
               <c:txPr>
-                <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
                   <a:spAutoFit/>
                 </a:bodyPr>
                 <a:lstStyle/>
@@ -5428,33 +5422,6 @@
             </c:dLbl>
             <c:dLbl>
               <c:idx val="4"/>
-              <c:numFmt formatCode="#,##0" sourceLinked="0"/>
-              <c:spPr>
-                <a:noFill/>
-                <a:ln>
-                  <a:noFill/>
-                </a:ln>
-                <a:effectLst/>
-              </c:spPr>
-              <c:txPr>
-                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-                  <a:spAutoFit/>
-                </a:bodyPr>
-                <a:lstStyle/>
-                <a:p>
-                  <a:pPr>
-                    <a:defRPr sz="1100" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                      <a:solidFill>
-                        <a:schemeClr val="tx1"/>
-                      </a:solidFill>
-                      <a:latin typeface="CMU Serif" panose="02000603000000000000" pitchFamily="2" charset="0"/>
-                      <a:ea typeface="CMU Serif" panose="02000603000000000000" pitchFamily="2" charset="0"/>
-                      <a:cs typeface="CMU Serif" panose="02000603000000000000" pitchFamily="2" charset="0"/>
-                    </a:defRPr>
-                  </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
-                </a:p>
-              </c:txPr>
               <c:dLblPos val="outEnd"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="1"/>
@@ -6129,10 +6096,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="5.982931774246783E-2"/>
-          <c:y val="9.8363702375819734E-2"/>
-          <c:w val="0.9328497909792679"/>
-          <c:h val="0.79500805554925236"/>
+          <c:x val="0.1039909943891744"/>
+          <c:y val="0.13600216590663519"/>
+          <c:w val="0.88868811589419594"/>
+          <c:h val="0.73652017741467035"/>
         </c:manualLayout>
       </c:layout>
       <c:barChart>
@@ -6175,13 +6142,13 @@
                 <a:effectLst/>
               </c:spPr>
               <c:txPr>
-                <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
                   <a:spAutoFit/>
                 </a:bodyPr>
                 <a:lstStyle/>
                 <a:p>
                   <a:pPr>
-                    <a:defRPr sz="1200" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                       <a:solidFill>
                         <a:schemeClr val="bg1"/>
                       </a:solidFill>
@@ -6208,6 +6175,12 @@
             </c:dLbl>
             <c:dLbl>
               <c:idx val="1"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-7.4850299401198151E-3"/>
+                  <c:y val="-2.2140223975387046E-3"/>
+                </c:manualLayout>
+              </c:layout>
               <c:dLblPos val="outEnd"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="1"/>
@@ -6224,6 +6197,12 @@
             </c:dLbl>
             <c:dLbl>
               <c:idx val="2"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-9.730538922155689E-3"/>
+                  <c:y val="2.2140223975386231E-3"/>
+                </c:manualLayout>
+              </c:layout>
               <c:dLblPos val="outEnd"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="1"/>
@@ -6253,7 +6232,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1200" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1"/>
                     </a:solidFill>
@@ -6376,13 +6355,13 @@
                 <a:effectLst/>
               </c:spPr>
               <c:txPr>
-                <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
                   <a:spAutoFit/>
                 </a:bodyPr>
                 <a:lstStyle/>
                 <a:p>
                   <a:pPr>
-                    <a:defRPr sz="1200" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                       <a:solidFill>
                         <a:schemeClr val="bg1"/>
                       </a:solidFill>
@@ -6441,6 +6420,12 @@
             </c:dLbl>
             <c:dLbl>
               <c:idx val="3"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-4.4910179640718561E-3"/>
+                  <c:y val="-3.3210335963080651E-2"/>
+                </c:manualLayout>
+              </c:layout>
               <c:dLblPos val="outEnd"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="1"/>
@@ -6457,6 +6442,12 @@
             </c:dLbl>
             <c:dLbl>
               <c:idx val="4"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="0"/>
+                  <c:y val="-5.535055993846761E-2"/>
+                </c:manualLayout>
+              </c:layout>
               <c:numFmt formatCode="#,##0" sourceLinked="0"/>
               <c:spPr>
                 <a:noFill/>
@@ -6472,7 +6463,7 @@
                 <a:lstStyle/>
                 <a:p>
                   <a:pPr>
-                    <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                       <a:solidFill>
                         <a:schemeClr val="tx1"/>
                       </a:solidFill>
@@ -6513,7 +6504,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1200" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1"/>
                     </a:solidFill>
@@ -6631,6 +6622,72 @@
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="5.988023952095781E-3"/>
+                  <c:y val="-2.2140223975387046E-3"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="outEnd"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000000-05C2-8040-96F4-116C4014A792}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="7.4850299401197605E-3"/>
+                  <c:y val="-2.2140223975387449E-3"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="outEnd"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000002-05C2-8040-96F4-116C4014A792}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="2"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="7.4850299401197605E-3"/>
+                  <c:y val="-2.2140223975387046E-3"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="outEnd"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000003-05C2-8040-96F4-116C4014A792}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
             <c:numFmt formatCode="#,##0" sourceLinked="0"/>
             <c:spPr>
               <a:noFill/>
@@ -6646,7 +6703,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1200" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1"/>
                     </a:solidFill>
@@ -6764,6 +6821,28 @@
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="5.988023952095781E-3"/>
+                  <c:y val="-2.2140223975387046E-3"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="outEnd"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000001-05C2-8040-96F4-116C4014A792}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
             <c:numFmt formatCode="#,##0" sourceLinked="0"/>
             <c:spPr>
               <a:noFill/>
@@ -6779,7 +6858,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1200" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1"/>
                     </a:solidFill>
@@ -6914,7 +6993,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="2400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -6966,7 +7045,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="3200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1">
                         <a:lumMod val="65000"/>
@@ -6979,7 +7058,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US" sz="1800" b="1" i="0">
+                  <a:rPr lang="en-US" sz="3200" b="0" i="0">
                     <a:latin typeface="CMU Serif" panose="02000603000000000000" pitchFamily="2" charset="0"/>
                     <a:ea typeface="CMU Serif" panose="02000603000000000000" pitchFamily="2" charset="0"/>
                     <a:cs typeface="CMU Serif" panose="02000603000000000000" pitchFamily="2" charset="0"/>
@@ -6989,6 +7068,14 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="6.8514545711726165E-4"/>
+              <c:y val="0.24386766106681196"/>
+            </c:manualLayout>
+          </c:layout>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -7002,7 +7089,7 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:defRPr sz="3200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
                     <a:schemeClr val="tx1">
                       <a:lumMod val="65000"/>
@@ -7034,7 +7121,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1200" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="2000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -7064,6 +7151,16 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="2.0477981045782464E-2"/>
+          <c:y val="0.87281049132769783"/>
+          <c:w val="0.97176858880663863"/>
+          <c:h val="0.11059971551390455"/>
+        </c:manualLayout>
+      </c:layout>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -7077,7 +7174,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+            <a:defRPr sz="2400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
@@ -11920,16 +12017,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>177800</xdr:colOff>
-      <xdr:row>118</xdr:row>
-      <xdr:rowOff>190500</xdr:rowOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>368300</xdr:colOff>
+      <xdr:row>125</xdr:row>
+      <xdr:rowOff>148167</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>22</xdr:col>
-      <xdr:colOff>635000</xdr:colOff>
-      <xdr:row>140</xdr:row>
-      <xdr:rowOff>127000</xdr:rowOff>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>152</xdr:row>
+      <xdr:rowOff>169333</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -12965,10 +13062,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{079671CB-D97D-EF41-AB2E-001CE763E275}">
-  <dimension ref="A3:V117"/>
+  <dimension ref="A3:V119"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A115" workbookViewId="0">
-      <selection activeCell="I145" sqref="I145"/>
+    <sheetView tabSelected="1" topLeftCell="A111" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="B123" sqref="B123"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -14347,7 +14444,7 @@
       </c>
       <c r="M104" s="4"/>
       <c r="N104">
-        <f t="shared" ref="N104:N107" si="1">-1*I104</f>
+        <f t="shared" ref="N104:N105" si="1">-1*I104</f>
         <v>37990.821387299999</v>
       </c>
       <c r="O104">
@@ -14458,7 +14555,7 @@
     <row r="110" spans="2:17" x14ac:dyDescent="0.2">
       <c r="N110" s="7"/>
     </row>
-    <row r="113" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A113" s="9" t="s">
         <v>41</v>
       </c>
@@ -14478,7 +14575,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="114" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A114" s="8" t="s">
         <v>42</v>
       </c>
@@ -14494,7 +14591,7 @@
       <c r="E114" s="4"/>
       <c r="F114" s="4"/>
     </row>
-    <row r="115" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
         <v>43</v>
       </c>
@@ -14514,7 +14611,7 @@
         <v>36157.299250999997</v>
       </c>
     </row>
-    <row r="116" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
         <v>55</v>
       </c>
@@ -14534,7 +14631,7 @@
         <v>35689.0869991</v>
       </c>
     </row>
-    <row r="117" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
         <v>56</v>
       </c>
@@ -14552,6 +14649,74 @@
       </c>
       <c r="F117" s="4">
         <v>6138.8505425499998</v>
+      </c>
+      <c r="G117">
+        <f>1-B117/B114</f>
+        <v>0.95924103485957168</v>
+      </c>
+      <c r="H117">
+        <f>1-C117/C114</f>
+        <v>0.80692328532906965</v>
+      </c>
+      <c r="I117">
+        <f>1-D117/D114</f>
+        <v>0.71993597017714983</v>
+      </c>
+      <c r="L117">
+        <f>AVERAGE(G117:I117)</f>
+        <v>0.82870009678859702</v>
+      </c>
+    </row>
+    <row r="118" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="G118">
+        <f>1-B117/B115</f>
+        <v>0.99110836586237583</v>
+      </c>
+      <c r="H118">
+        <f t="shared" ref="H118:K118" si="2">1-C117/C115</f>
+        <v>0.84159339748987883</v>
+      </c>
+      <c r="I118">
+        <f t="shared" si="2"/>
+        <v>0.81544776958071807</v>
+      </c>
+      <c r="J118">
+        <f t="shared" si="2"/>
+        <v>0.77128245882441859</v>
+      </c>
+      <c r="K118">
+        <f t="shared" si="2"/>
+        <v>0.83021822233085563</v>
+      </c>
+      <c r="L118">
+        <f>AVERAGE(G118:K118)</f>
+        <v>0.84993004281764928</v>
+      </c>
+    </row>
+    <row r="119" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="G119">
+        <f>1-B117/B116</f>
+        <v>0.40446731922490864</v>
+      </c>
+      <c r="H119">
+        <f t="shared" ref="H119:K119" si="3">1-C117/C116</f>
+        <v>0.79226105982706052</v>
+      </c>
+      <c r="I119">
+        <f t="shared" si="3"/>
+        <v>0.68763042470316971</v>
+      </c>
+      <c r="J119">
+        <f t="shared" si="3"/>
+        <v>0.76393946212898278</v>
+      </c>
+      <c r="K119">
+        <f t="shared" si="3"/>
+        <v>0.82799082132011925</v>
+      </c>
+      <c r="L119">
+        <f>AVERAGE(G119:K119)</f>
+        <v>0.69525781744084814</v>
       </c>
     </row>
   </sheetData>

</xml_diff>